<commit_message>
[Shubham]Updated code on 27/12/23
</commit_message>
<xml_diff>
--- a/data/excel/OtherMiscFunctionality1.xlsx
+++ b/data/excel/OtherMiscFunctionality1.xlsx
@@ -1,15 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B896ED7F-980F-4C32-A499-EFBF4C4582B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Flight" sheetId="1" r:id="rId1"/>
     <sheet name="Hotel" sheetId="2" r:id="rId2"/>
     <sheet name="All" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="113">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -165,13 +167,208 @@
   </si>
   <si>
     <t>Laxmi@1234</t>
+  </si>
+  <si>
+    <t>//test.quadlabs.net/backoffice/</t>
+  </si>
+  <si>
+    <t>Quad@721</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>DynamicHeader</t>
+  </si>
+  <si>
+    <t>OTHERS</t>
+  </si>
+  <si>
+    <t>DHeadTitle</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>HeadDescription</t>
+  </si>
+  <si>
+    <t>HeadOnType</t>
+  </si>
+  <si>
+    <t>ApplyLevel</t>
+  </si>
+  <si>
+    <t>NoOfHeaders</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>01,02</t>
+  </si>
+  <si>
+    <t>Test1,Test2</t>
+  </si>
+  <si>
+    <t>DropDown</t>
+  </si>
+  <si>
+    <t>Corporate</t>
+  </si>
+  <si>
+    <t>DataCaptureSource</t>
+  </si>
+  <si>
+    <t>Dynamic Element</t>
+  </si>
+  <si>
+    <t>DDisplayName</t>
+  </si>
+  <si>
+    <t>Test1</t>
+  </si>
+  <si>
+    <t>DProductType</t>
+  </si>
+  <si>
+    <t>DCaptureEvent</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>OBT</t>
+  </si>
+  <si>
+    <t>Booking</t>
+  </si>
+  <si>
+    <t>BookingF</t>
+  </si>
+  <si>
+    <t>Destination</t>
+  </si>
+  <si>
+    <t>CorporateF</t>
+  </si>
+  <si>
+    <t>Account No. (Auto Capture)</t>
+  </si>
+  <si>
+    <t>Corporate Branch</t>
+  </si>
+  <si>
+    <t>CorporateBranchF</t>
+  </si>
+  <si>
+    <t>Alt. Branch Code (Auto Capture)</t>
+  </si>
+  <si>
+    <t>Corporate Cost Center</t>
+  </si>
+  <si>
+    <t>CorporateCostF</t>
+  </si>
+  <si>
+    <t>Cost Center Code (Auto Capture)</t>
+  </si>
+  <si>
+    <t>CorporateFareF</t>
+  </si>
+  <si>
+    <t>Corporate Project</t>
+  </si>
+  <si>
+    <t>CorporateProjectF</t>
+  </si>
+  <si>
+    <t>Project Code (Auto Capture)</t>
+  </si>
+  <si>
+    <t>Corporate User Visa Details</t>
+  </si>
+  <si>
+    <t>CorporateUserF</t>
+  </si>
+  <si>
+    <t>Visa Country (Auto Capture)</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>DepartmentF</t>
+  </si>
+  <si>
+    <t>Designation</t>
+  </si>
+  <si>
+    <t>ManageDynamicHeads</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>ManageDataCapture</t>
+  </si>
+  <si>
+    <t>Air Reason Code</t>
+  </si>
+  <si>
+    <t>Test_All</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Test MO 2</t>
+  </si>
+  <si>
+    <t>Test MO 3</t>
+  </si>
+  <si>
+    <t>Test MO 4</t>
+  </si>
+  <si>
+    <t>Test MO 5</t>
+  </si>
+  <si>
+    <t>Test MO 6</t>
+  </si>
+  <si>
+    <t>Test MO 7</t>
+  </si>
+  <si>
+    <t>Test MO 8</t>
+  </si>
+  <si>
+    <t>Test MO 9</t>
+  </si>
+  <si>
+    <t>Test MO 10</t>
+  </si>
+  <si>
+    <t>Verify Dynamic element &amp; Data capture</t>
+  </si>
+  <si>
+    <t>Verify Data capture</t>
+  </si>
+  <si>
+    <t>Corporate Fare Denied Reasons</t>
+  </si>
+  <si>
+    <t>Department Email (Auto Capture)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,6 +386,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -268,7 +471,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -276,9 +479,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -560,7 +762,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -616,31 +818,31 @@
       <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="7" t="s">
         <v>30</v>
       </c>
     </row>
@@ -669,16 +871,16 @@
       <c r="H2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="8" t="s">
         <v>21</v>
       </c>
       <c r="M2">
@@ -702,35 +904,35 @@
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Laxmi@123"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"saurav_at"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"at"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"Positive,Negative"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"Flight,Hotel,All"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"Flight,Hotel"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H2" r:id="rId2" display="Shekhar123@"/>
+    <hyperlink ref="G2" r:id="rId1" display="shubham.natkar@quadlabs.com" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="H2" r:id="rId2" display="Shekhar123@" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -786,31 +988,31 @@
       <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="7" t="s">
         <v>30</v>
       </c>
     </row>
@@ -839,16 +1041,16 @@
       <c r="H2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="8" t="s">
         <v>23</v>
       </c>
       <c r="M2">
@@ -872,39 +1074,39 @@
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Flight,Hotel"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Flight,Hotel,All"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"Positive,Negative"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>"at"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{00000000-0002-0000-0100-000004000000}">
       <formula1>"saurav_at"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{00000000-0002-0000-0100-000005000000}">
       <formula1>"Laxmi@123"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H2" r:id="rId2" display="Shekhar123@"/>
+    <hyperlink ref="G2" r:id="rId1" display="shubham.natkar@quadlabs.com" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="H2" r:id="rId2" display="Shekhar123@" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -962,52 +1164,52 @@
       <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="T1" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="U1" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="V1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="W1" s="10" t="s">
+      <c r="W1" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="X1" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Y1" s="7" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1036,16 +1238,16 @@
       <c r="H2" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="8" t="s">
         <v>21</v>
       </c>
       <c r="M2">
@@ -1090,37 +1292,1769 @@
     </row>
   </sheetData>
   <dataValidations count="9">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Laxmi@1234"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"saurav_at"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>"at"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{00000000-0002-0000-0200-000003000000}">
       <formula1>"Positive,Negative"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2" xr:uid="{00000000-0002-0000-0200-000004000000}">
       <formula1>"Flight,Hotel,All"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2" xr:uid="{00000000-0002-0000-0200-000005000000}">
       <formula1>"Flight,Hotel"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2" xr:uid="{00000000-0002-0000-0200-000006000000}">
       <formula1>"Agreement Fee,Agreement Markup"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2 X2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2 X2" xr:uid="{00000000-0002-0000-0200-000007000000}">
       <formula1>"% (Percent),% Markup,Fixed Amount"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2 Y2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2 Y2" xr:uid="{00000000-0002-0000-0200-000008000000}">
       <formula1>"Base Fare,Base Fare + Tax,Base Fare + YQ,Base Fare + YQ+YR,Net Fare(Tax Inclusive),Net Fare(Tax Exclusive)"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H2" r:id="rId2" display="Shekhar123@"/>
+    <hyperlink ref="G2" r:id="rId1" display="shubham.natkar@quadlabs.com" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="H2" r:id="rId2" display="Shekhar123@" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6BC3D69-7098-4745-AD6E-6852F4C82A3D}">
+  <dimension ref="A1:AU11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="AS16" sqref="AS16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12" customWidth="1"/>
+    <col min="39" max="42" width="16.42578125" customWidth="1"/>
+    <col min="43" max="43" width="14.7109375" customWidth="1"/>
+    <col min="44" max="44" width="12.140625" customWidth="1"/>
+    <col min="45" max="45" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AM1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AN1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO1" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AP1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AR1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="AS1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AT1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AU1" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" s="4">
+        <v>2</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" s="4">
+        <v>2</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>2</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="T2" s="4">
+        <v>10</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="W2" s="4">
+        <v>10</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF2" s="4">
+        <v>2</v>
+      </c>
+      <c r="AG2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI2" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="AJ2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK2" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="AM2" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AN2" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="AO2" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="AP2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AQ2" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AR2" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="AS2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AT2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AU2" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="4">
+        <v>2</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" s="4">
+        <v>2</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>2</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="T3" s="4">
+        <v>10</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="W3" s="4">
+        <v>10</v>
+      </c>
+      <c r="X3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z3" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB3" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD3" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF3" s="4">
+        <v>2</v>
+      </c>
+      <c r="AG3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI3" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="AJ3" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AK3" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL3" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="AM3" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AN3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="AO3" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="AP3" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AQ3" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AR3" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="AS3" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AT3" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AU3" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" s="4">
+        <v>2</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O4" s="4">
+        <v>2</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>2</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="T4" s="4">
+        <v>10</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="V4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="W4" s="4">
+        <v>10</v>
+      </c>
+      <c r="X4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z4" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB4" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC4" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD4" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE4" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF4" s="4">
+        <v>2</v>
+      </c>
+      <c r="AG4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI4" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="AJ4" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK4" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL4" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="AM4" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AN4" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="AO4" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="AP4" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AQ4" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AR4" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="AS4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AT4" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AU4" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" s="4">
+        <v>2</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O5" s="4">
+        <v>2</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>2</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="T5" s="4">
+        <v>10</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="V5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="W5" s="4">
+        <v>10</v>
+      </c>
+      <c r="X5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z5" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB5" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC5" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD5" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE5" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF5" s="4">
+        <v>2</v>
+      </c>
+      <c r="AG5" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI5" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="AJ5" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="AK5" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL5" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="AM5" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AN5" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="AO5" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="AP5" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AQ5" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AR5" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="AS5" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AT5" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AU5" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M6" s="4">
+        <v>2</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O6" s="4">
+        <v>2</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>2</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="T6" s="4">
+        <v>10</v>
+      </c>
+      <c r="U6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="V6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="W6" s="4">
+        <v>10</v>
+      </c>
+      <c r="X6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z6" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA6" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB6" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD6" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE6" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF6" s="4">
+        <v>2</v>
+      </c>
+      <c r="AG6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI6" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="AJ6" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK6" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL6" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="AM6" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AN6" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="AO6" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="AP6" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AQ6" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AR6" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="AS6" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AT6" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AU6" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M7" s="4">
+        <v>2</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O7" s="4">
+        <v>2</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>2</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="T7" s="4">
+        <v>10</v>
+      </c>
+      <c r="U7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="V7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="W7" s="4">
+        <v>10</v>
+      </c>
+      <c r="X7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z7" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB7" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD7" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE7" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF7" s="4">
+        <v>2</v>
+      </c>
+      <c r="AG7" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH7" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI7" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="AJ7" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AK7" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL7" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="AM7" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AN7" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="AO7" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="AP7" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AQ7" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AR7" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="AS7" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AT7" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AU7" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M8" s="4">
+        <v>2</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O8" s="4">
+        <v>2</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>2</v>
+      </c>
+      <c r="R8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="T8" s="4">
+        <v>10</v>
+      </c>
+      <c r="U8" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="V8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="W8" s="4">
+        <v>10</v>
+      </c>
+      <c r="X8" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z8" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB8" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC8" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD8" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE8" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF8" s="4">
+        <v>2</v>
+      </c>
+      <c r="AG8" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH8" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI8" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="AJ8" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AK8" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL8" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="AM8" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AN8" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="AO8" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="AP8" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AQ8" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AR8" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="AS8" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AT8" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AU8" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M9" s="4">
+        <v>2</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O9" s="4">
+        <v>2</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>2</v>
+      </c>
+      <c r="R9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="T9" s="4">
+        <v>10</v>
+      </c>
+      <c r="U9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="V9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="W9" s="4">
+        <v>10</v>
+      </c>
+      <c r="X9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z9" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA9" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB9" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC9" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD9" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE9" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF9" s="4">
+        <v>2</v>
+      </c>
+      <c r="AG9" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI9" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="AJ9" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AK9" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL9" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="AM9" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AN9" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="AO9" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="AP9" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AQ9" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AR9" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="AS9" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AT9" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AU9" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M10" s="4">
+        <v>2</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O10" s="4">
+        <v>2</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>2</v>
+      </c>
+      <c r="R10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="T10" s="4">
+        <v>10</v>
+      </c>
+      <c r="U10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="V10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="W10" s="4">
+        <v>10</v>
+      </c>
+      <c r="X10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z10" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA10" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB10" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC10" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD10" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE10" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF10" s="4">
+        <v>2</v>
+      </c>
+      <c r="AG10" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH10" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI10" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="AJ10" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK10" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL10" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="AM10" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AN10" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="AO10" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="AP10" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AQ10" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AR10" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="AS10" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AT10" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AU10" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M11" s="4">
+        <v>2</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O11" s="4">
+        <v>2</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>2</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="T11" s="4">
+        <v>10</v>
+      </c>
+      <c r="U11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="V11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="W11" s="4">
+        <v>10</v>
+      </c>
+      <c r="X11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z11" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA11" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB11" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC11" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD11" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE11" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF11" s="4">
+        <v>2</v>
+      </c>
+      <c r="AG11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH11" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI11" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="AJ11" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="AK11" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL11" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="AM11" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AN11" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="AO11" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="AP11" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AQ11" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AR11" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="AS11" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AT11" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AU11" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <dataValidations count="25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y2:Y11 V2:V11" xr:uid="{7D63E4F2-ED2E-4C8B-A783-1B51599E1CDC}">
+      <formula1>"Base Fare,Base Fare + Tax,Base Fare + YQ,Base Fare + YQ+YR,Net Fare(Tax Inclusive),Net Fare(Tax Exclusive)"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2:X11 U2:U11" xr:uid="{6F7E5691-0B42-49B4-B3E2-1F2811BB9279}">
+      <formula1>"% (Percent),% Markup,Fixed Amount"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S11" xr:uid="{9F2C1181-8C5A-4C80-8A17-05ED9353315E}">
+      <formula1>"Agreement Fee,Agreement Markup"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L11" xr:uid="{54725ADE-F270-4E68-91DA-1AD93600E841}">
+      <formula1>"Flight,Hotel"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K11" xr:uid="{C5251248-E5F2-4C6E-AD9D-6957CA6294C9}">
+      <formula1>"Flight,Hotel,All"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B11" xr:uid="{1C2A374F-92BA-4187-BE79-1B1A6BD28E98}">
+      <formula1>"Positive,Negative"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F11" xr:uid="{DA3B347C-9E2F-4471-9EEC-5A189F297992}">
+      <formula1>"at"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G11" xr:uid="{94BE5398-BCE1-41F7-817B-115098381FB6}">
+      <formula1>"saurav_at"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H11" xr:uid="{49174F2A-3AB7-448B-B55A-0DFBBA7E528E}">
+      <formula1>"Laxmi@1234,Quad@721"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA2:AA11" xr:uid="{3FADD4D4-2501-426F-85FE-07C58D1CAA4B}">
+      <formula1>"CAR REASON CODES,INSURANCE REASON CODES,MARHABA REASON CODES,NO HOTEL REASON CODES,OTHER PRODUCT REASON CODES,RAIL REASON CODES,TRANSFER REASON CODES,VISA REASON CODES,REASON CODE,TRIP PURPOSE,TRIP APPROVAL,TRIP APPROVER,BOOKERS NAME,LLA FARE,OTHERS"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD2:AD11" xr:uid="{02AA7772-990F-41E8-8EF9-A3DD2CBDF535}">
+      <formula1>"DropDown,Text"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE2:AE11" xr:uid="{8D6C5CE0-C903-4C52-A456-D3020E4CFAFC}">
+      <formula1>"Transaction,Corporate,Traveller"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ2:AJ6 AJ8:AJ11" xr:uid="{D28A7AA5-6EAE-4D3C-9D1B-8F2147CEDCEE}">
+      <formula1>"Booking,Corporate,Corporate Branch,Corporate Cost Center,Corporate Fare Denied  Reasons,Corporate Project,Corporate User Visa Details,Department,Designation,Division,Dynamic Element,Flight Information(D),Grade Level,Host Branch,Host Business Unit"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AT2:AT11" xr:uid="{4D717076-8BC9-4472-9794-710C81651F3D}">
+      <formula1>"Air,Hotel,Others"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AU2:AU11" xr:uid="{77045CC2-8E2F-423A-9037-F7A10BC8FA8A}">
+      <formula1>"Quotation,Booking,Ticket,OBT"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK2:AK11" xr:uid="{C626AB9B-5BE3-49A6-8FE8-3578ADAB6F67}">
+      <formula1>"Destination"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL2:AL11" xr:uid="{4521E87B-E603-402A-A1DF-C9BAD1804585}">
+      <formula1>"Account No. (Auto Capture),Customer Number (Auto Capture),Alternate Reference Code (Auto Capture),City (Auto Capture),Corporate Name (Auto Capture),Company Security Code (Auto Capture),Country (Auto Capture),PlatformID (Auto Capture)"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2:AM11" xr:uid="{93E25753-543D-4727-A985-FEA4980121E6}">
+      <formula1>"Alt. Branch Code (Auto Capture),Branch Address1 (Auto Capture),Branch Code (Auto Capture),City Name (Auto Capture),Country Code (Auto Capture),Post Code (Auto Capture),State (Auto Capture)"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN2:AN11" xr:uid="{997CABB1-BD39-4BDC-81A9-76C368B2564F}">
+      <formula1>"Cost Center Code (Auto Capture),Cost Centre Name"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO2:AO11" xr:uid="{766B9898-C769-4DE6-A0B9-E23411011324}">
+      <formula1>"Air Reason Code,Hotel Reason Code"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP2:AP11" xr:uid="{6715DA18-6412-475A-AEE5-683DBE015F5A}">
+      <formula1>"Project Code (Auto Capture),Project Name (Auto Capture)"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ2:AQ11" xr:uid="{FA63C410-66A4-45E8-A6B9-E027C6F75D89}">
+      <formula1>"Visa Country (Auto Capture),Visa Number (Auto Capture),Visa POI (Auto Capture),Visa Remark (Auto Capture),Visa Type (Auto Capture),VisaValidaty EndDate (Auto Capture),VisaValidity StartDate (Auto Capture)"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI2:AI11 Z2:Z11" xr:uid="{C8C62FBC-68AB-4BF7-80BF-9CF95E8478E6}">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ7" xr:uid="{D9238E23-E720-49BF-92CC-A7314F0BE8F5}">
+      <formula1>"Booking,Corporate,Corporate Branch,Corporate Cost Center,Corporate Fare Denied Reasons,Corporate Project,Corporate User Visa Details,Department,Designation,Division,Dynamic Element,Flight Information(D),Grade Level,Host Branch,Host Business Unit"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR2:AR11" xr:uid="{2110CF3E-3044-49B4-8B4F-28A9187633F4}">
+      <formula1>"Department Email (Auto Capture),Dept Head UserId  (Auto Capture),Department Name (Auto Capture),Department Phone No (Auto Capture)"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" display="shubham.natkar@quadlabs.com" xr:uid="{37283775-BBD1-49A3-ADC1-03C05EBA5EAA}"/>
+    <hyperlink ref="H2" r:id="rId2" display="Shekhar123@" xr:uid="{B2C3F32D-0835-4B47-B757-BEEE57E4FB3B}"/>
+    <hyperlink ref="G3" r:id="rId3" display="shubham.natkar@quadlabs.com" xr:uid="{7D103D20-D50C-47A1-9E77-DDFD06D2EC93}"/>
+    <hyperlink ref="H3" r:id="rId4" display="Shekhar123@" xr:uid="{388DE9F5-63E1-47D2-8E89-135D05057188}"/>
+    <hyperlink ref="G4" r:id="rId5" display="shubham.natkar@quadlabs.com" xr:uid="{161F0828-3F4D-4040-976D-D858CEF825C9}"/>
+    <hyperlink ref="H4" r:id="rId6" display="Shekhar123@" xr:uid="{AA2DD494-987A-4295-AE2B-5D145E248ADD}"/>
+    <hyperlink ref="G5" r:id="rId7" display="shubham.natkar@quadlabs.com" xr:uid="{D9D899F5-5E6B-4D66-A19B-43413C91EDC5}"/>
+    <hyperlink ref="H5" r:id="rId8" display="Shekhar123@" xr:uid="{F0A8993B-B2BD-4CDF-A558-6548DB6853CD}"/>
+    <hyperlink ref="G6" r:id="rId9" display="shubham.natkar@quadlabs.com" xr:uid="{49CC67D8-520A-4ACA-B549-A8DC41B05A3D}"/>
+    <hyperlink ref="H6" r:id="rId10" display="Shekhar123@" xr:uid="{CB016F9E-48AC-4FE6-9DA8-12E9391D483E}"/>
+    <hyperlink ref="G7" r:id="rId11" display="shubham.natkar@quadlabs.com" xr:uid="{FDBB8D4F-A3DA-45BB-BC35-AF96C1C491AC}"/>
+    <hyperlink ref="H7" r:id="rId12" display="Shekhar123@" xr:uid="{E3243A9C-7881-4362-974D-C8EDADE21F24}"/>
+    <hyperlink ref="G8" r:id="rId13" display="shubham.natkar@quadlabs.com" xr:uid="{B2D6040B-F934-4E1E-8A37-2C3059E350DD}"/>
+    <hyperlink ref="H8" r:id="rId14" display="Shekhar123@" xr:uid="{3797762E-D338-475C-A27A-2349294685EC}"/>
+    <hyperlink ref="G9" r:id="rId15" display="shubham.natkar@quadlabs.com" xr:uid="{C3B931E7-0726-4246-A1D4-7C0DC076344D}"/>
+    <hyperlink ref="H9" r:id="rId16" display="Shekhar123@" xr:uid="{55310877-685E-42E1-9110-29102B80818B}"/>
+    <hyperlink ref="G10" r:id="rId17" display="shubham.natkar@quadlabs.com" xr:uid="{B67ABF1D-F8A5-4034-91B8-6A40F161C652}"/>
+    <hyperlink ref="H10" r:id="rId18" display="Shekhar123@" xr:uid="{5E7F1CCB-32B7-4F19-8701-27BA46341807}"/>
+    <hyperlink ref="G11" r:id="rId19" display="shubham.natkar@quadlabs.com" xr:uid="{4486CEBD-4337-40E5-B8AB-8CEDEACA646F}"/>
+    <hyperlink ref="H11" r:id="rId20" display="Shekhar123@" xr:uid="{2DF1B454-2ADE-41F5-9484-AFBE49CEFE21}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>